<commit_message>
updated excel sheet for inserting teachers
</commit_message>
<xml_diff>
--- a/server/samplesheets/sampleDataTeacher.xlsx
+++ b/server/samplesheets/sampleDataTeacher.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10608"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\WEB\vamshi\NIEPID\server\samplesheets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nandanagulavancha/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3E6BF05F-8279-48C1-AF27-9DD3D78D2CF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5D86722-E6BC-C24C-AC51-058BA7F25ACA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{F52E085B-39B7-486D-A62F-120619D618FB}"/>
+    <workbookView xWindow="1240" yWindow="500" windowWidth="23260" windowHeight="12460" xr2:uid="{F52E085B-39B7-486D-A62F-120619D618FB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,28 +36,31 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
-    <t>teacherId</t>
+    <t>TeacherId</t>
   </si>
   <si>
-    <t>teacherName</t>
+    <t>Name</t>
   </si>
   <si>
-    <t>teacherMNo</t>
+    <t>MobileNo</t>
   </si>
   <si>
-    <t>email</t>
+    <t>Email</t>
   </si>
   <si>
-    <t>classId</t>
+    <t>ClassId</t>
+  </si>
+  <si>
+    <t>NOTE: Only use one of the following values for classId: 'preprimary_1', 'preprimary_2', 'preprimary_3', 'primary1_1', 'primary1_2', 'primary1_3', 'primary2_1', 'primary2_2', 'primary2_3'</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -73,8 +76,21 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Aptos Narrow (Body)"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -84,6 +100,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -97,14 +119,23 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -437,39 +468,54 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8932A90C-3AE0-4CF2-A6F2-707823902E36}">
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="15.33203125" customWidth="1"/>
-    <col min="2" max="2" width="25.5546875" customWidth="1"/>
+    <col min="2" max="2" width="25.5" customWidth="1"/>
     <col min="3" max="3" width="22.6640625" customWidth="1"/>
     <col min="4" max="4" width="34.6640625" customWidth="1"/>
-    <col min="5" max="5" width="22.44140625" customWidth="1"/>
+    <col min="5" max="5" width="45.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E2" s="1" t="s">
         <v>4</v>
       </c>
     </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D3" s="2"/>
+    </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:E1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>